<commit_message>
Update: Modify input_test.xlsx to surpress a message in process_raw_data()
</commit_message>
<xml_diff>
--- a/inst/input_test.xlsx
+++ b/inst/input_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="212">
   <si>
     <t>牛舎間の移動の設定</t>
     <rPh sb="0" eb="2">
@@ -951,10 +951,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ハッチ</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1028,10 +1024,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>搾乳</t>
     <rPh sb="0" eb="2">
       <t>サク</t>
@@ -1056,10 +1048,6 @@
   </si>
   <si>
     <t>milking</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>s</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -2809,9 +2797,6 @@
       <c r="F5" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="M5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2831,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>14</v>
@@ -2855,10 +2840,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>14</v>
@@ -2879,10 +2861,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>19</v>
@@ -2903,10 +2882,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="M9" s="11" t="s">
         <v>28</v>
@@ -2930,10 +2906,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="M10" s="11" t="s">
         <v>28</v>
@@ -2960,10 +2933,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>14</v>
@@ -2983,13 +2953,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N12" s="11">
         <v>2</v>
@@ -3009,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
@@ -3018,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J13" s="52">
         <v>41919</v>
@@ -3041,10 +3008,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="M14" s="11" t="s">
         <v>23</v>
@@ -3518,11 +3482,8 @@
       <c r="F5" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="N5" s="11">
         <v>1</v>
@@ -3546,22 +3507,22 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="N6" s="11">
         <v>5</v>
       </c>
       <c r="R6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3576,20 +3537,17 @@
         <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N7" s="11">
         <v>8</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3604,10 +3562,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>81</v>
@@ -3616,10 +3571,10 @@
         <v>13</v>
       </c>
       <c r="R8" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="S8" s="37" t="s">
         <v>127</v>
-      </c>
-      <c r="S8" s="37" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3634,13 +3589,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="N9" s="11">
         <v>1</v>
@@ -3649,10 +3601,10 @@
         <v>1</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -3667,13 +3619,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N10" s="11">
         <v>7</v>
@@ -3685,10 +3634,10 @@
         <v>1</v>
       </c>
       <c r="R10" s="46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -3703,13 +3652,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I11" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="N11" s="11">
         <v>3</v>
@@ -3718,7 +3664,7 @@
         <v>74</v>
       </c>
       <c r="S11" s="49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -3732,13 +3678,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N12" s="11">
         <v>2</v>
@@ -3748,7 +3691,7 @@
       </c>
       <c r="R12" s="50"/>
       <c r="S12" s="51" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -3762,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
@@ -3771,19 +3714,19 @@
         <v>2</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J13" s="52">
         <v>41919</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N13" s="11">
         <v>4</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="S13" s="21" t="s">
         <v>2</v>
@@ -3800,13 +3743,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N14" s="11">
         <v>3</v>
@@ -3815,31 +3755,31 @@
         <v>74</v>
       </c>
       <c r="S14" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="R15" s="13"/>
       <c r="S15" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="R16" s="13"/>
       <c r="S16" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="18:19">
       <c r="R17" s="13"/>
       <c r="S17" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="18:19">
       <c r="R18" s="17"/>
       <c r="S18" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="18:19">
@@ -3852,46 +3792,46 @@
     </row>
     <row r="20" spans="18:19">
       <c r="R20" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="18:19">
       <c r="R21" s="13"/>
       <c r="S21" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="18:19">
       <c r="R22" s="13"/>
       <c r="S22" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="18:19">
       <c r="R23" s="13"/>
       <c r="S23" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="18:19">
       <c r="R24" s="13"/>
       <c r="S24" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="18:19">
       <c r="R25" s="13"/>
       <c r="S25" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="18:19">
       <c r="R26" s="17"/>
       <c r="S26" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="18:19">
@@ -3907,36 +3847,36 @@
         <v>74</v>
       </c>
       <c r="S28" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="18:19">
       <c r="R29" s="13"/>
       <c r="S29" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="18:19">
       <c r="R30" s="13"/>
       <c r="S30" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="18:19">
       <c r="R31" s="13"/>
       <c r="S31" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="18:19">
       <c r="R32" s="17"/>
       <c r="S32" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="18:19">
       <c r="R33" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>2</v>
@@ -3944,21 +3884,21 @@
     </row>
     <row r="34" spans="18:19">
       <c r="R34" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S34" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="18:19">
       <c r="R35" s="17"/>
       <c r="S35" s="19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="18:19">
       <c r="R36" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>2</v>
@@ -3966,27 +3906,27 @@
     </row>
     <row r="37" spans="18:19">
       <c r="R37" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="18:19">
       <c r="R38" s="13"/>
       <c r="S38" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="18:19">
       <c r="R39" s="17"/>
       <c r="S39" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="18:19">
       <c r="R40" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>2</v>
@@ -3994,21 +3934,21 @@
     </row>
     <row r="41" spans="18:19">
       <c r="R41" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="18:19">
       <c r="R42" s="17"/>
       <c r="S42" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="18:19">
       <c r="R43" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>2</v>
@@ -4019,13 +3959,13 @@
         <v>74</v>
       </c>
       <c r="S44" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="18:19">
       <c r="R45" s="17"/>
       <c r="S45" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="18:19">
@@ -4038,33 +3978,33 @@
     </row>
     <row r="47" spans="18:19">
       <c r="R47" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="18:19">
       <c r="R48" s="13"/>
       <c r="S48" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="18:19">
       <c r="R49" s="13"/>
       <c r="S49" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="18:19">
       <c r="R50" s="17"/>
       <c r="S50" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="18:19">
       <c r="R51" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>2</v>
@@ -4072,22 +4012,22 @@
     </row>
     <row r="52" spans="18:19">
       <c r="R52" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="18:19">
       <c r="R53" s="13"/>
       <c r="S53" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="18:19">
       <c r="R54" s="17"/>
       <c r="S54" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="18:19">
@@ -4100,45 +4040,45 @@
     </row>
     <row r="56" spans="18:19">
       <c r="R56" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="18:19">
       <c r="R57" s="13"/>
       <c r="S57" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="18:19">
       <c r="R58" s="13"/>
       <c r="S58" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="18:19">
       <c r="R59" s="13"/>
       <c r="S59" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="18:19">
       <c r="R60" s="13"/>
       <c r="S60" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="18:19">
       <c r="R61" s="17"/>
       <c r="S61" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="18:19">
       <c r="R62" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S62" s="21" t="s">
         <v>2</v>
@@ -4149,19 +4089,19 @@
         <v>74</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="18:19">
       <c r="R64" s="13"/>
       <c r="S64" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="18:19">
       <c r="R65" s="17"/>
       <c r="S65" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="18:19">
@@ -4177,13 +4117,13 @@
         <v>74</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="18:19">
       <c r="R68" s="17"/>
       <c r="S68" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="18:19">
@@ -4196,21 +4136,21 @@
     </row>
     <row r="70" spans="18:19">
       <c r="R70" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="18:19">
       <c r="R71" s="17"/>
       <c r="S71" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="18:19">
       <c r="R72" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S72" s="21" t="s">
         <v>2</v>
@@ -4221,19 +4161,19 @@
         <v>74</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="18:19">
       <c r="R74" s="13"/>
       <c r="S74" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="18:19">
       <c r="R75" s="13"/>
       <c r="S75" s="16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="18:19">
@@ -4246,10 +4186,10 @@
     </row>
     <row r="77" spans="18:19">
       <c r="R77" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S77" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="18:19">
@@ -4262,28 +4202,28 @@
     </row>
     <row r="79" spans="18:19">
       <c r="R79" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="18:19">
       <c r="R80" s="13"/>
       <c r="S80" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="18:19">
       <c r="R81" s="13"/>
       <c r="S81" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="18:19">
       <c r="R82" s="17"/>
       <c r="S82" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="18:19">
@@ -4296,40 +4236,40 @@
     </row>
     <row r="84" spans="18:19">
       <c r="R84" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="S84" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="18:19">
       <c r="R85" s="13"/>
       <c r="S85" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="18:19">
       <c r="R86" s="13"/>
       <c r="S86" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="18:19">
       <c r="R87" s="13"/>
       <c r="S87" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="18:19">
       <c r="R88" s="13"/>
       <c r="S88" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" spans="18:19">
       <c r="R89" s="17"/>
       <c r="S89" s="19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4422,7 +4362,7 @@
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4643,7 +4583,7 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4801,7 +4741,7 @@
     <row r="25" spans="6:7">
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="6:7">
@@ -4823,7 +4763,7 @@
     <row r="28" spans="6:7">
       <c r="F28" s="13"/>
       <c r="G28" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="6:7">

</xml_diff>

<commit_message>
Update: Add a comment to input_test.xlsx
</commit_message>
<xml_diff>
--- a/inst/input_test.xlsx
+++ b/inst/input_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="12795"/>
+    <workbookView xWindow="4050" yWindow="0" windowWidth="28035" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cow" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="213">
   <si>
     <t>牛舎間の移動の設定</t>
     <rPh sb="0" eb="2">
@@ -1946,6 +1946,22 @@
     </rPh>
     <rPh sb="65" eb="66">
       <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※新生子牛用牛舎</t>
+    <rPh sb="1" eb="3">
+      <t>アラオイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウシ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ギュウシャ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -2154,7 +2170,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2312,6 +2328,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2617,7 +2636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -3028,9 +3047,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3093,6 +3112,9 @@
       </c>
       <c r="C5" s="11" t="s">
         <v>71</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:7">

</xml_diff>

<commit_message>
Clean: Move a selected cell in input_test.xlsx
</commit_message>
<xml_diff>
--- a/inst/input_test.xlsx
+++ b/inst/input_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="0" windowWidth="28035" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="4050" yWindow="0" windowWidth="28035" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="cow" sheetId="5" r:id="rId1"/>
@@ -2636,7 +2636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -3047,9 +3047,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>